<commit_message>
feat: Update dependencies and add networkx to requirements.txt
</commit_message>
<xml_diff>
--- a/excel_data.xlsx
+++ b/excel_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajos\Structure-Alvaro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5718A5E5-811E-4007-9B8B-C9BEE51F3A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB15F31-55FC-445F-B313-F4BC04F91FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A7FA216E-B6EC-432F-A3FC-9FC43E578A6A}"/>
   </bookViews>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40940666-1A44-46CC-9B18-93697FA53828}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,6 +482,31 @@
         <v>76</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>